<commit_message>
added excel plate 2
</commit_message>
<xml_diff>
--- a/data/fig5-6_migration/Transwell_migration_pdgf_plate_2.xlsx
+++ b/data/fig5-6_migration/Transwell_migration_pdgf_plate_2.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordi Camps\stack\PhD\Results\Chemokine in muscular dystrophy project\Chemokines in muscular dystrophy project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0099120\stack\PhD\Results\Chemokine in muscular dystrophy project\Chemokines in muscular dystrophy project\data\fig5-6_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0FAF84B-B0A1-4456-9A45-391398667AFA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="1200" windowWidth="14940" windowHeight="9150"/>
+    <workbookView xWindow="2685" yWindow="1200" windowWidth="14940" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="112">
   <si>
     <t>compound</t>
   </si>
@@ -353,6 +352,9 @@
   </si>
   <si>
     <t>thirty_percent_FBS</t>
+  </si>
+  <si>
+    <t>Plate</t>
   </si>
 </sst>
 </file>
@@ -391,7 +393,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -669,2551 +671,2842 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94:B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>1995</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>231</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.95</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>590</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>108</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1933</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>623</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>8.2100000000000009</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1642</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3.28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1868</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>592</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>8.07</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1614</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3.23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>108</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>2049</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>876</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>10.9</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>2180</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <v>2016</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>154</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1.95</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>390</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>109</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>2058</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>240</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2.97</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>594</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2094</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1484</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>18.100000000000001</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>3620</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>7.24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
         <v>109</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1955</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>223</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2.91</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>582</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>110</v>
       </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10">
         <v>1451</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1018</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>17.899999999999999</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3580</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>7.16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
         <v>110</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1919</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>7965</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>106</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>21200</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>42.4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1962</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>5012</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>65.099999999999994</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>13020</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
         <v>110</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1816</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>9961</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>140</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>28000</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>108</v>
       </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14">
         <v>2027</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>460</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>5.78</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1156</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2.31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>3</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>1858</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>292</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>4</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>800</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1.6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>108</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>1995</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>547</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>6.98</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1396</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>2.79</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>108</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>1880</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>1389</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>18.8</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>3760</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>7.52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
         <v>109</v>
       </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18">
         <v>2065</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>167</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>2.06</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>412</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.82</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
         <v>109</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>2004</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>358</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>4.55</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>910</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>1.82</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
         <v>109</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>2011</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>1477</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>18.7</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>3740</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>7.48</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
         <v>109</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>2021</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>948</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>11.9</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>2380</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>4.76</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>110</v>
       </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22">
         <v>1886</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>1768</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>23.9</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>4780</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>9.56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>1798</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>8168</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>116</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>23200</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>46.4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
         <v>110</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>1937</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>3375</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>44.4</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>8880</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>17.8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
         <v>110</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>1954</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>8716</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>114</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>22800</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>45.6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
         <v>108</v>
       </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26">
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26">
         <v>1944</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>256</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>3.35</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>670</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>1.34</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
         <v>108</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>3</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>1879</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>237</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>3.21</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>642</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>1.28</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
         <v>108</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>1956</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>635</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>8.27</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>1654</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>3.31</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
         <v>108</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>1998</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>568</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>7.24</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>1448</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>2.9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
         <v>109</v>
       </c>
-      <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30">
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30">
         <v>1855</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>138</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>1.9</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>380</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>0.76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
         <v>109</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>1846</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>429</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>5.92</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>1184</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>2.37</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
         <v>109</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>4</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>1915</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>1308</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>17.399999999999999</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>3480</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>6.96</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
         <v>109</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>1888</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>1147</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>15.5</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>3100</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>6.2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
         <v>110</v>
       </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34">
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34">
         <v>1974</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>1708</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>22</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>4400</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>45</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
         <v>110</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>3</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>1954</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>7505</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>97.8</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>19560</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>39.1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
         <v>110</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>4</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>1863</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>4483</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>61.3</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>12260</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>24.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
         <v>110</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>5</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>1940</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>10939</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>144</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>28800</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>57.6</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
         <v>108</v>
       </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38">
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38">
         <v>1964</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>147</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>1.91</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>382</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>0.76</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
         <v>108</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>3</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>1883</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>283</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>3.83</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>766</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>1.53</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
         <v>108</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>4</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>1925</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>348</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>4.6100000000000003</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>922</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>1.84</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
         <v>108</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>5</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>1893</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>1338</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>18</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>3600</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>7.2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
         <v>109</v>
       </c>
-      <c r="C42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42">
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42">
         <v>1955</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>101</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>1.32</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>264</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>0.53</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
         <v>109</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>3</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>1845</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>338</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>4.67</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>934</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>1.87</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
         <v>109</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>4</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>1982</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>873</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>11.2</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>2240</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
         <v>109</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>5</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>2081</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>703</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>8.61</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>1722</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>3.44</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
         <v>110</v>
       </c>
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46">
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46">
         <v>1904</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>1911</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>25.6</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>5120</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
         <v>110</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>3</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>1719</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>8312</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>123</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>24600</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>49.2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
         <v>110</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>4</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>1891</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>5080</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>68.400000000000006</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>13680</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>27.4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>59</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
         <v>110</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>1883</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>10583</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>143</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>28600</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>57.2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>60</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
         <v>108</v>
       </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50">
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50">
         <v>1882</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>95</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>1.29</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>258</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>0.52</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
         <v>108</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>3</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>3198</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>182</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>1.45</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>290</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>62</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
         <v>108</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>4</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>1914</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>287</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>3.82</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>764</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>1.53</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>63</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
         <v>108</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>5</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>2013</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>1693</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>21.4</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>4280</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>8.56</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
         <v>109</v>
       </c>
-      <c r="C54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54">
+      <c r="D54" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54">
         <v>1993</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>86</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>220</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>0.44</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>65</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
         <v>109</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>3</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>2071</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>166</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>2.04</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>408</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>0.82</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>66</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
         <v>109</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>4</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>2066</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>746</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>1840</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>3.68</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
         <v>109</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>5</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>2016</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>377</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>4.76</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>952</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>1.9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>68</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
         <v>110</v>
       </c>
-      <c r="C58" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58">
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58">
         <v>1930</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>1556</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>20.5</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>4100</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>69</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
         <v>110</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>3</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>1745</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>7136</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>104</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>20800</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>41.6</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>70</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
         <v>110</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>4</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>1857</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>5483</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>75.2</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>15040</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>30.1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>71</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
         <v>110</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>5</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>1792</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>10622</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>151</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>30200</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>60.4</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>72</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
         <v>108</v>
       </c>
-      <c r="C62" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62">
+      <c r="D62" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62">
         <v>1937</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>119</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>1.57</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>314</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>0.63</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>73</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
         <v>108</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>3</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>1890</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>157</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>2.12</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>424</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>0.85</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>74</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
         <v>108</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>4</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>1952</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>217</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>2.83</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>566</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>75</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
         <v>108</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>5</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>1975</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>760</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>1960</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>3.92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>76</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
         <v>109</v>
       </c>
-      <c r="C66" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66">
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66">
         <v>1868</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>99</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>1.35</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>270</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>0.54</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>77</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
         <v>109</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>3</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>1813</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>111</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>1.56</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>312</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>0.62</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>78</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
         <v>109</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>4</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>1803</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>867</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>12.3</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>2460</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>4.92</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
         <v>109</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>5</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>1931</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>442</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>5.83</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>1166</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>2.33</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>80</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
         <v>110</v>
       </c>
-      <c r="C70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70">
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70">
         <v>1753</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>2598</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>37.799999999999997</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>7560</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>15.1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>81</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
         <v>110</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>3</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>1802</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>9526</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>135</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>27000</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>82</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
         <v>110</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>4</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>1925</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>6914</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>91.5</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>18300</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>36.6</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>83</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
         <v>110</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>5</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>2027</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>11131</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>140</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>28000</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>84</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
         <v>108</v>
       </c>
-      <c r="C74" t="s">
-        <v>2</v>
-      </c>
-      <c r="D74">
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74">
         <v>1820</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>94</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>1.32</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>264</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>0.53</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>85</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
         <v>108</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>3</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>1920</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>161</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>2.14</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>428</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>0.86</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>86</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
         <v>108</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>4</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>1892</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>260</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>3.5</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>700</v>
       </c>
-      <c r="H76">
+      <c r="I76">
         <v>1.4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>87</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
         <v>108</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>5</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>2046</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>154</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>1.92</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>384</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>0.77</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>88</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
         <v>109</v>
       </c>
-      <c r="C78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D78">
+      <c r="D78" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78">
         <v>1913</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>93</v>
       </c>
-      <c r="F78" s="1">
-        <f>(E78*5)/(D78*195)*1095</f>
+      <c r="G78" s="1">
+        <f>(F78*5)/(E78*195)*1095</f>
         <v>1.3649523503156542</v>
       </c>
-      <c r="G78" s="2">
-        <f>F78*195</f>
+      <c r="H78" s="2">
+        <f>G78*195</f>
         <v>266.16570831155258</v>
       </c>
-      <c r="H78" s="1">
-        <f>G78/50000*100</f>
+      <c r="I78" s="1">
+        <f>H78/50000*100</f>
         <v>0.53233141662310512</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>89</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
         <v>109</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>3</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>1941</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>116</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>1.52</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>304</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>0.61</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>90</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
         <v>109</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>4</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>1864</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>745</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>10.199999999999999</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>2040</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>4.08</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>91</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
         <v>109</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>5</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>1883</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>611</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>8.27</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>1654</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>3.31</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>92</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
         <v>110</v>
       </c>
-      <c r="C82" t="s">
-        <v>2</v>
-      </c>
-      <c r="D82">
+      <c r="D82" t="s">
+        <v>2</v>
+      </c>
+      <c r="E82">
         <v>1786</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>2876</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>41</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>8200</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>93</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
         <v>110</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>3</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>1822</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>6534</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>91.4</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>18280</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <v>36.6</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>94</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
         <v>110</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>4</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>1902</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>6606</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>88.5</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>17700</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>35.4</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>95</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
         <v>110</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>5</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>1904</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>10500</v>
       </c>
-      <c r="F85" s="1">
-        <f>(E85*5)/(D85*195)*1095</f>
+      <c r="G85" s="1">
+        <f>(F85*5)/(E85*195)*1095</f>
         <v>154.83597285067873</v>
       </c>
-      <c r="G85" s="2">
-        <f>F85*195</f>
+      <c r="H85" s="2">
+        <f>G85*195</f>
         <v>30193.014705882353</v>
       </c>
-      <c r="H85" s="1">
-        <f>G85/50000*100</f>
+      <c r="I85" s="1">
+        <f>H85/50000*100</f>
         <v>60.38602941176471</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>96</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
         <v>108</v>
       </c>
-      <c r="C86" t="s">
-        <v>2</v>
-      </c>
-      <c r="D86">
+      <c r="D86" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86">
         <v>1751</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>92</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>1.34</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>268</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>0.54</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>97</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
         <v>108</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>3</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>1838</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>77</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>1.07</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>214</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>0.43</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>98</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
         <v>108</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>4</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>1826</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>154</v>
       </c>
-      <c r="F88">
+      <c r="G88">
         <v>2.15</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>430</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>0.86</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>99</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
         <v>108</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>5</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>1765</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>150</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>2.17</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>434</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>0.87</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>100</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
         <v>109</v>
       </c>
-      <c r="C90" t="s">
-        <v>2</v>
-      </c>
-      <c r="D90">
+      <c r="D90" t="s">
+        <v>2</v>
+      </c>
+      <c r="E90">
         <v>1744</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>185</v>
       </c>
-      <c r="F90">
+      <c r="G90">
         <v>2.7</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>540</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <v>1.08</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>101</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
         <v>109</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>3</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>1901</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>246</v>
       </c>
-      <c r="F91">
+      <c r="G91">
         <v>3.3</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>660</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <v>1.32</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>102</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
         <v>109</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>4</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>1755</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>384</v>
       </c>
-      <c r="F92">
+      <c r="G92">
         <v>5.57</v>
       </c>
-      <c r="G92">
+      <c r="H92">
         <v>1114</v>
       </c>
-      <c r="H92">
+      <c r="I92">
         <v>2.23</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>103</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
         <v>109</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>5</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>1804</v>
       </c>
-      <c r="E93">
+      <c r="F93">
         <v>842</v>
       </c>
-      <c r="F93">
+      <c r="G93">
         <v>11.9</v>
       </c>
-      <c r="G93">
+      <c r="H93">
         <v>2380</v>
       </c>
-      <c r="H93">
+      <c r="I93">
         <v>4.76</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>104</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
         <v>110</v>
       </c>
-      <c r="C94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D94">
+      <c r="D94" t="s">
+        <v>2</v>
+      </c>
+      <c r="E94">
         <v>1709</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>2879</v>
       </c>
-      <c r="F94">
+      <c r="G94">
         <v>42.9</v>
       </c>
-      <c r="G94">
+      <c r="H94">
         <v>8580</v>
       </c>
-      <c r="H94">
+      <c r="I94">
         <v>17.2</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>105</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
         <v>110</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>3</v>
       </c>
-      <c r="D95">
+      <c r="E95">
         <v>1666</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>5833</v>
       </c>
-      <c r="F95">
+      <c r="G95">
         <v>89.2</v>
       </c>
-      <c r="G95">
+      <c r="H95">
         <v>17840</v>
       </c>
-      <c r="H95">
+      <c r="I95">
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>106</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
         <v>110</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>4</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>1645</v>
       </c>
-      <c r="E96">
+      <c r="F96">
         <v>5423</v>
       </c>
-      <c r="F96">
+      <c r="G96">
         <v>84</v>
       </c>
-      <c r="G96">
+      <c r="H96">
         <v>16800</v>
       </c>
-      <c r="H96">
+      <c r="I96">
         <v>33.6</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>107</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
         <v>110</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>5</v>
       </c>
-      <c r="D97">
+      <c r="E97">
         <v>1633</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>8987</v>
       </c>
-      <c r="F97">
+      <c r="G97">
         <v>140</v>
       </c>
-      <c r="G97">
+      <c r="H97">
         <v>28000</v>
       </c>
-      <c r="H97">
+      <c r="I97">
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>